<commit_message>
updated xlsx file with aj
</commit_message>
<xml_diff>
--- a/exceldata.xlsx
+++ b/exceldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajay1\Desktop\repo\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF2963B-5899-4DF6-8C07-CDB92894095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC150914-4610-4C67-B52D-D1DAF523B1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{58BE7A49-456C-4100-8841-EDF235E98BEA}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TestCases</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>divya</t>
+  </si>
+  <si>
+    <t>ajay</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCCF677-C890-4140-BC11-4E5AD5B50C1F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,6 +559,11 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated xlsx file with ayvid
</commit_message>
<xml_diff>
--- a/exceldata.xlsx
+++ b/exceldata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajay1\Desktop\repo\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC150914-4610-4C67-B52D-D1DAF523B1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F96DA7-5B96-4B94-812E-9481E3316557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{58BE7A49-456C-4100-8841-EDF235E98BEA}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TestCases</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>ajay</t>
+  </si>
+  <si>
+    <t>ayvid</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCCF677-C890-4140-BC11-4E5AD5B50C1F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,6 +567,11 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>